<commit_message>
Completed data cleaning, augmentation, and rounding phases
</commit_message>
<xml_diff>
--- a/data/measurement_relationships.xlsx
+++ b/data/measurement_relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\my_project\body-measurement-predictor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0492A-127B-4EE2-A5B3-7452B347BDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF2B0EC-9F8A-49C0-A207-8D2430AD432D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t>Tolerance</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Turtleneck standard</t>
   </si>
   <si>
-    <t>Balanced figure standard (±1cm)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cropped trouser standard   </t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Wide-leg trouser standard</t>
   </si>
   <si>
-    <t>Balanced body type standard</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Health assessment guideline (WHO)</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t xml:space="preserve">Long-sleeve garment standard </t>
   </si>
   <si>
-    <t>Bodice balance tolerance</t>
-  </si>
-  <si>
     <t>Menswear standard ±0.8cm</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>Low-rise trouser standard</t>
   </si>
   <si>
-    <t>Spinal curvature adjustment</t>
-  </si>
-  <si>
     <t>Bra cup spacing standard</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t xml:space="preserve"> Skinny jean standard</t>
   </si>
   <si>
-    <t>Standard hourglass tolerance</t>
-  </si>
-  <si>
     <t>Sleeve mobility allowance</t>
   </si>
   <si>
@@ -264,12 +249,6 @@
     <t>skirt_full_length_cm = 0.5 * height_cm</t>
   </si>
   <si>
-    <t xml:space="preserve"> elbow_length_cm = 0.25 * height_cm</t>
-  </si>
-  <si>
-    <t>bust_height_cm = 1.5 * front_waist_length_cm</t>
-  </si>
-  <si>
     <t>bust_height_cm = 0.6 * bust_cm</t>
   </si>
   <si>
@@ -291,15 +270,9 @@
     <t>skirt_knee_length_cm = 0.6 * skirt_full_length_cm</t>
   </si>
   <si>
-    <t>back_waist_length_cm = 0.9 * front_waist_length_cm</t>
-  </si>
-  <si>
     <t>around_wrist_cm = 0.05 * height_cm</t>
   </si>
   <si>
-    <t>bust_cm = 1.2 * waist_cm</t>
-  </si>
-  <si>
     <t>around_armhole_cm = 0.3 * bust_cm</t>
   </si>
   <si>
@@ -381,16 +354,13 @@
     <t>bust_cm = 1.5 * waist_cm</t>
   </si>
   <si>
-    <t>around_thigh_cm = 0.6 * waist_cm</t>
-  </si>
-  <si>
-    <t>hip_cm = 5 + bust_cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hip_cm = 5 +  bust_cm </t>
-  </si>
-  <si>
     <t>chest_cm = 10  + waist_cm</t>
+  </si>
+  <si>
+    <t>elbow_length_cm = 0.25 * height_cm</t>
+  </si>
+  <si>
+    <t>around_thigh_cm = 0.35 * height_cm</t>
   </si>
 </sst>
 </file>
@@ -709,9 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -722,18 +694,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -744,7 +716,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>0.03</v>
@@ -755,7 +727,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -766,7 +738,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>1.2</v>
@@ -777,7 +749,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>1.5</v>
@@ -788,7 +760,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>0.8</v>
@@ -799,7 +771,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>1.5</v>
@@ -810,7 +782,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <v>0.02</v>
@@ -821,7 +793,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <v>0.4</v>
@@ -832,150 +804,150 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>0.03</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B14">
         <v>0.5</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B15">
         <v>0.02</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>0.03</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>0.3</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B20">
         <v>0.1</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>0.02</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B22">
         <v>0.03</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B23">
         <v>0.02</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B24">
         <v>0.1</v>
@@ -986,408 +958,353 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B25">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B26">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="B27">
-        <v>0.8</v>
+        <v>0.02</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B28">
-        <v>0.02</v>
+        <v>0.5</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B29">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B30">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B31">
         <v>0.01</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B33">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B34">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B35">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="B36">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B37">
-        <v>0.01</v>
+        <v>0.4</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B38">
         <v>0.3</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B39">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B40">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B41">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B43">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B44">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B45">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B46">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B47">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C47" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B48">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B49">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B50">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B51">
         <v>0.02</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B53">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C53" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B55">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B56">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>105</v>
-      </c>
-      <c r="B57">
-        <v>0.02</v>
-      </c>
-      <c r="C57" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58">
-        <v>0.05</v>
-      </c>
-      <c r="C58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59">
-        <v>0.01</v>
-      </c>
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60">
-        <v>0.02</v>
-      </c>
-      <c r="C60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>109</v>
-      </c>
-      <c r="B61">
-        <v>0.01</v>
-      </c>
-      <c r="C61" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>